<commit_message>
make edits based on new data
</commit_message>
<xml_diff>
--- a/data/Copy of 2023_Wild Winter STHD_All_Sorel.xlsx
+++ b/data/Copy of 2023_Wild Winter STHD_All_Sorel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa.sharepoint.com/sites/DFW-TeamFPColumbiaRiverManagementUnit953/Shared Documents/Data and Analysis Tools/Run Reconstruction/Steelhead/RProject_run_recon_forecast_winter_steelhead/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{DBAC2A32-ADDD-4020-9E3B-0FACA769C051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C807C845-03EB-48CC-916A-53E0EAE5DA28}"/>
+  <xr:revisionPtr revIDLastSave="42" documentId="8_{DBAC2A32-ADDD-4020-9E3B-0FACA769C051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A799FC9B-B983-4D68-80DE-5E87F3BC9E3F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{129475E2-A35E-4D6E-B5FC-E639465237AF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{129475E2-A35E-4D6E-B5FC-E639465237AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Lower Gorge Summary_2023" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Lower Gorge Tribs - Estimated Total Winter Steelhead Escapement</t>
   </si>
@@ -144,22 +144,13 @@
     <t>Gray_PC</t>
   </si>
   <si>
-    <t>Coweeman</t>
-  </si>
-  <si>
-    <t>Elochoman-Skamokawa</t>
-  </si>
-  <si>
-    <t>Grays-Chinook</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Green River (NF Toutle) </t>
-  </si>
-  <si>
     <t>Lower Gorge (Columbia)</t>
   </si>
   <si>
     <t>Escapement</t>
+  </si>
+  <si>
+    <t>Kalama</t>
   </si>
 </sst>
 </file>
@@ -3887,10 +3878,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A593AD5E-7F35-4A75-8B4F-B83142DAA280}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3906,7 +3897,7 @@
         <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
         <v>20</v>
@@ -3919,8 +3910,8 @@
       <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="9">
-        <v>526</v>
+      <c r="C2" s="10">
+        <v>94</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -3931,96 +3922,12 @@
         <v>2023</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="9">
-        <v>234</v>
+        <v>24</v>
+      </c>
+      <c r="C3" s="10">
+        <v>609</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>2023</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="9">
-        <v>342</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>2023</v>
-      </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="9">
-        <v>752</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>2023</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="9">
-        <v>330</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>2023</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="9">
-        <v>258</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>2023</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="9">
-        <v>370</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>2023</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="10">
-        <v>94</v>
-      </c>
-      <c r="D9" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>